<commit_message>
Corregi un error en la tabla dinamica y el error de la lectura de fechas desde excel
</commit_message>
<xml_diff>
--- a/src/assets/docs/registro_usuarios.xlsx
+++ b/src/assets/docs/registro_usuarios.xlsx
@@ -46,10 +46,10 @@
     <t>Carrera</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Correo</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,10 +405,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Integre la funcion de inscribirse y salir de un proyecto
</commit_message>
<xml_diff>
--- a/src/assets/docs/registro_usuarios.xlsx
+++ b/src/assets/docs/registro_usuarios.xlsx
@@ -389,7 +389,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,16 +405,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>

</xml_diff>